<commit_message>
Update the monitoring form for the fourth week dated 21/02/2024
</commit_message>
<xml_diff>
--- a/JudahAriesakaMagaini/Judah.xlsx
+++ b/JudahAriesakaMagaini/Judah.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kuliah\semester 8\ta\Ontologi-Sejarah-Indonesia\JudahAriesakaMagaini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FEB7C2-7C5A-42B6-B93D-01BCECBCC853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09CD4BC-D0D3-405D-89DD-9083D101D258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="135">
   <si>
     <t>Monitoring Skripsi dari:</t>
   </si>
@@ -519,6 +519,25 @@
 https://id.wikipedia.org/wiki/Templat:Sejarah_konflik_di_Indonesia 
 - Menemukan library baru pywikibot untuk melakukan scrapping halaman Wikipedia per kategori, template, ataupun judul dalam bahasa Indonesia dan Inggris.
 - Mengumpulkan data judul dan infobox yang terkait ke dalam suatu file csv.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alokasi waktu: 12 jam
+Link Commit: https://github.com/rcsenlia/Ontologi-Sejarah-Indonesia/commit/1476eb1ca301d2e1df46dadaf44d0a68ad1ebc68
+Uraian:
+- Mengeksplorasi dan menemukan kategori baru halaman pada Wikipedia yang relevan dengan sejarah Indonesia periode Orde Baru.
+https://id.wikipedia.org/wiki/Kategori:Pendirian_di_Indonesia_menurut_tahun
+- Mengumpulkan jenis-jenis infobox dari data-data yang telah diambil dari Wikipedia
+- Untuk setiap jenis infobox, dilakukan mapping dari key menjadi kolom dan dari value menjadi baris dan ditulis ke dalam file CSV.
+</t>
+  </si>
+  <si>
+    <t>TODO:
+- Mengeksplorasi tech stack yang akan digunakan untuk menyimpan data triple.
+- Mengeksplorasi tech stack yang akan digunakan untuk memvisualisasikan data berdasarkan ruang, waktu, dan peristiwa (aktor).
+- Mencoba membuat ontologi dengan menggunakan SEM.</t>
+  </si>
+  <si>
+    <t>Data gathering diselesaikan dahulu untuk mulai ke tahap konstruksi model ontologi. Data gathering selanjutnya bisa dilakukan secara iteratif. Untuk selanjutnya, fokus kepada tech stack untuk menyimpan data triple dan memvisualisasikannya melalui aplikasi.</t>
   </si>
 </sst>
 </file>
@@ -1114,10 +1133,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1126,12 +1151,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1410,10 +1429,10 @@
   <dimension ref="A1:AE1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="8" topLeftCell="E13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1423,8 +1442,8 @@
     <col min="3" max="3" width="7.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="8" width="40.7109375" customWidth="1"/>
-    <col min="9" max="20" width="17.85546875" customWidth="1"/>
+    <col min="6" max="9" width="40.7109375" customWidth="1"/>
+    <col min="10" max="20" width="17.85546875" customWidth="1"/>
     <col min="21" max="21" width="19.28515625" customWidth="1"/>
     <col min="22" max="23" width="16.5703125" customWidth="1"/>
   </cols>
@@ -1434,7 +1453,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="94" t="s">
+      <c r="C1" s="97" t="s">
         <v>120</v>
       </c>
       <c r="D1" s="95"/>
@@ -1466,7 +1485,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="96" t="s">
+      <c r="C2" s="98" t="s">
         <v>121</v>
       </c>
       <c r="D2" s="95"/>
@@ -1625,7 +1644,7 @@
       <c r="B7" s="4"/>
       <c r="C7" s="15"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="97"/>
+      <c r="E7" s="99"/>
       <c r="F7" s="95"/>
       <c r="G7" s="95"/>
       <c r="H7" s="95"/>
@@ -1728,7 +1747,7 @@
       <c r="AD8" s="15"/>
       <c r="AE8" s="4"/>
     </row>
-    <row r="9" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="19"/>
       <c r="B9" s="19" t="s">
         <v>26</v>
@@ -1951,7 +1970,9 @@
       <c r="H12" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="I12" s="24"/>
+      <c r="I12" s="24" t="s">
+        <v>123</v>
+      </c>
       <c r="J12" s="24"/>
       <c r="K12" s="25"/>
       <c r="L12" s="24"/>
@@ -1992,7 +2013,9 @@
       <c r="H13" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="I13" s="24"/>
+      <c r="I13" s="23" t="s">
+        <v>134</v>
+      </c>
       <c r="J13" s="24"/>
       <c r="K13" s="24"/>
       <c r="L13" s="24"/>
@@ -2036,7 +2059,7 @@
         <v>131</v>
       </c>
       <c r="I14" s="23" t="s">
-        <v>32</v>
+        <v>132</v>
       </c>
       <c r="J14" s="23" t="s">
         <v>32</v>
@@ -2085,7 +2108,7 @@
       <c r="AD14" s="4"/>
       <c r="AE14" s="4"/>
     </row>
-    <row r="15" spans="1:31" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="19" t="s">
         <v>33</v>
@@ -2098,7 +2121,9 @@
       <c r="H15" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="I15" s="24"/>
+      <c r="I15" s="23" t="s">
+        <v>133</v>
+      </c>
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
       <c r="L15" s="24"/>
@@ -2300,7 +2325,7 @@
       <c r="AE19" s="4"/>
     </row>
     <row r="20" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="98" t="s">
+      <c r="A20" s="100" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="95"/>
@@ -2649,7 +2674,7 @@
       <c r="AE24" s="4"/>
     </row>
     <row r="25" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="98" t="s">
+      <c r="A25" s="100" t="s">
         <v>44</v>
       </c>
       <c r="B25" s="95"/>
@@ -2817,7 +2842,7 @@
       <c r="AE28" s="4"/>
     </row>
     <row r="29" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="99" t="s">
+      <c r="A29" s="94" t="s">
         <v>51</v>
       </c>
       <c r="B29" s="95"/>
@@ -4651,7 +4676,7 @@
       <c r="AE52" s="4"/>
     </row>
     <row r="53" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="100" t="s">
+      <c r="A53" s="96" t="s">
         <v>75</v>
       </c>
       <c r="B53" s="95"/>
@@ -36084,6 +36109,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update the monitoring form for the fifth week dated 28/02/2024
</commit_message>
<xml_diff>
--- a/JudahAriesakaMagaini/Judah.xlsx
+++ b/JudahAriesakaMagaini/Judah.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kuliah\semester 8\ta\Ontologi-Sejarah-Indonesia\JudahAriesakaMagaini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09CD4BC-D0D3-405D-89DD-9083D101D258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6FE27E-525B-4758-B49D-DCD5B82BDFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Monitoring" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="138">
   <si>
     <t>Monitoring Skripsi dari:</t>
   </si>
@@ -539,6 +539,71 @@
   <si>
     <t>Data gathering diselesaikan dahulu untuk mulai ke tahap konstruksi model ontologi. Data gathering selanjutnya bisa dilakukan secara iteratif. Untuk selanjutnya, fokus kepada tech stack untuk menyimpan data triple dan memvisualisasikannya melalui aplikasi.</t>
   </si>
+  <si>
+    <t>SEM ontology dapat digunakan sebagai core dengan beberapa pertimbangan tambahan, seperti untuk time bisa menggunakan time ontology agar lebih detail (https://www.w3.org/TR/owl-time/#overview). Selanjutnya untuk type bisa langsung menjadi subclass Event ataupun Actor, sehingga tidak perlu menggunakan ActorType dan sejenisnya. Untuk place pada SEM masih bersifat abstrak sehingga dapat menggunakan GeoSPARQL sebagai pertimbangan (https://www.ogc.org/standard/geosparql/). Untuk role sebagai constraint memiliki banyak fungsi, misalnya korban, attacker, atau jabatan dalam suatu organisasi. Untuk database yang akan digunakan, dapat mengeksplor AllegroDB ataupun GraphDB ataupun neo4j. Terakhir, untuk visualisasi peta, dapat mencoba untuk menggunakan OpenStreetMap dan pembagian province berdasarkan periode waktunya.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TODO:
+- Mencoba beberapa database untuk kemudian ditentukan </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">pros </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">dan </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cons</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sebagai pertimbangan untuk database yang akan digunakan.
+- Membuat mockup visualisasi untuk disajikan kepada orang sejarah.</t>
+    </r>
+  </si>
+  <si>
+    <t>Alokasi waktu: 16 jam 
+Link Commit: https://github.com/rcsenlia/Ontologi-Sejarah-Indonesia/commit/b6655c49e39b8821493210e67fe2f8da44a36ab6
+Uraian:
+- Mengeksplorasi visualisasi peta untuk menampilkan data sejarah.
+- Mengimplementasikan visualisasi peta dengan React menggunakan library leaflet.
+- Mempelajari SEM ontology dan mulai mengembangkan ontologi tersebut sesuai dengan data orde baru yang diperoleh.
+- Mengeksplorasi database yang akan digunakan dan mencoba menggunakan Blazegraph pada local dengan melakukan running melalui terminal.
+cara menjalankan server:
+1. java -server -Xmx4g -jar blazegraph.jar
+2. java -cp blazegraph.jar com.bigdata.rdf.store.DataLoader -namespace myNamespace fastload.properties spotify_top_chart.ttl
+3. curl -X POST http://localhost:9999/blazegraph/sparql --data-urlencode "query=PREFIX : &lt;http://domain.org/ns/&gt; SELECT * WHERE { ?p rdf:type :Song }"</t>
+  </si>
 </sst>
 </file>
 
@@ -547,7 +612,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d&quot;-&quot;mmm&quot;-&quot;yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -597,6 +662,21 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -864,7 +944,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1133,6 +1213,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1429,10 +1512,10 @@
   <dimension ref="A1:AE1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="8" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="8" topLeftCell="I13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1442,8 +1525,8 @@
     <col min="3" max="3" width="7.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="9" width="40.7109375" customWidth="1"/>
-    <col min="10" max="20" width="17.85546875" customWidth="1"/>
+    <col min="6" max="10" width="40.7109375" customWidth="1"/>
+    <col min="11" max="20" width="17.85546875" customWidth="1"/>
     <col min="21" max="21" width="19.28515625" customWidth="1"/>
     <col min="22" max="23" width="16.5703125" customWidth="1"/>
   </cols>
@@ -1453,10 +1536,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="98" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="95"/>
+      <c r="D1" s="96"/>
       <c r="J1" s="3"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -1485,10 +1568,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="98" t="s">
+      <c r="C2" s="99" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="95"/>
+      <c r="D2" s="96"/>
       <c r="J2" s="3"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
@@ -1644,12 +1727,12 @@
       <c r="B7" s="4"/>
       <c r="C7" s="15"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="95"/>
-      <c r="I7" s="95"/>
-      <c r="J7" s="95"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="96"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -1973,7 +2056,9 @@
       <c r="I12" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="J12" s="24"/>
+      <c r="J12" s="24" t="s">
+        <v>123</v>
+      </c>
       <c r="K12" s="25"/>
       <c r="L12" s="24"/>
       <c r="M12" s="24"/>
@@ -1996,7 +2081,7 @@
       <c r="AD12" s="4"/>
       <c r="AE12" s="4"/>
     </row>
-    <row r="13" spans="1:31" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" ht="255" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="19" t="s">
         <v>30</v>
@@ -2016,7 +2101,9 @@
       <c r="I13" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="J13" s="24"/>
+      <c r="J13" s="24" t="s">
+        <v>135</v>
+      </c>
       <c r="K13" s="24"/>
       <c r="L13" s="24"/>
       <c r="M13" s="24"/>
@@ -2039,7 +2126,7 @@
       <c r="AD13" s="4"/>
       <c r="AE13" s="4"/>
     </row>
-    <row r="14" spans="1:31" ht="331.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="19" t="s">
         <v>31</v>
@@ -2062,7 +2149,7 @@
         <v>132</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>32</v>
+        <v>137</v>
       </c>
       <c r="K14" s="23" t="s">
         <v>32</v>
@@ -2124,7 +2211,9 @@
       <c r="I15" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="J15" s="24"/>
+      <c r="J15" s="94" t="s">
+        <v>136</v>
+      </c>
       <c r="K15" s="24"/>
       <c r="L15" s="24"/>
       <c r="M15" s="24"/>
@@ -2325,10 +2414,10 @@
       <c r="AE19" s="4"/>
     </row>
     <row r="20" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="100" t="s">
+      <c r="A20" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="95"/>
+      <c r="B20" s="96"/>
       <c r="C20" s="17"/>
       <c r="D20" s="18"/>
       <c r="E20" s="18" t="s">
@@ -2674,10 +2763,10 @@
       <c r="AE24" s="4"/>
     </row>
     <row r="25" spans="1:31" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="95"/>
+      <c r="B25" s="96"/>
       <c r="C25" s="17"/>
       <c r="D25" s="37"/>
       <c r="E25" s="37"/>
@@ -2842,10 +2931,10 @@
       <c r="AE28" s="4"/>
     </row>
     <row r="29" spans="1:31" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="94" t="s">
+      <c r="A29" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="95"/>
+      <c r="B29" s="96"/>
       <c r="C29" s="37"/>
       <c r="D29" s="18" t="s">
         <v>6</v>
@@ -4676,12 +4765,12 @@
       <c r="AE52" s="4"/>
     </row>
     <row r="53" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="96" t="s">
+      <c r="A53" s="97" t="s">
         <v>75</v>
       </c>
-      <c r="B53" s="95"/>
-      <c r="C53" s="95"/>
-      <c r="D53" s="95"/>
+      <c r="B53" s="96"/>
+      <c r="C53" s="96"/>
+      <c r="D53" s="96"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
       <c r="G53" s="10"/>
@@ -4711,10 +4800,10 @@
       <c r="AE53" s="4"/>
     </row>
     <row r="54" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="95"/>
-      <c r="B54" s="95"/>
-      <c r="C54" s="95"/>
-      <c r="D54" s="95"/>
+      <c r="A54" s="96"/>
+      <c r="B54" s="96"/>
+      <c r="C54" s="96"/>
+      <c r="D54" s="96"/>
       <c r="E54" s="10"/>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
@@ -4744,10 +4833,10 @@
       <c r="AE54" s="4"/>
     </row>
     <row r="55" spans="1:31" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="95"/>
-      <c r="B55" s="95"/>
-      <c r="C55" s="95"/>
-      <c r="D55" s="95"/>
+      <c r="A55" s="96"/>
+      <c r="B55" s="96"/>
+      <c r="C55" s="96"/>
+      <c r="D55" s="96"/>
       <c r="E55" s="10"/>
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>

</xml_diff>

<commit_message>
Update the monitoring for the seventh week dated 13/03/2024
</commit_message>
<xml_diff>
--- a/JudahAriesakaMagaini/Judah.xlsx
+++ b/JudahAriesakaMagaini/Judah.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kuliah\semester 8\ta\Ontologi-Sejarah-Indonesia\JudahAriesakaMagaini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A340AADF-C766-45CE-B901-8FE27D708979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA3352D-0A75-4EE8-821E-4739BF4083C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="145">
   <si>
     <t>Monitoring Skripsi dari:</t>
   </si>
@@ -617,6 +617,28 @@
   </si>
   <si>
     <t>Database/triplestore yang akan digunakan adalah GraphDB yang memiliki visualisasi triple yang dapat memudahkan pengembang dalam melakukan debugging. Untuk tahap berikutnya, membuat rancangan ontologi/vocabulary dengan SEM sebagai dasar yang didukung dengan ontologi time, GeoSPARQL, Dublin Core, dan lainnya. Selain itu, aplikasi visualisasi akan dikembangkan dan diintegrasikan dengan prioritas timeline, peta, dan graph.</t>
+  </si>
+  <si>
+    <t>Data lokasi latitude dan longitude yang diperoleh dengan geopy belum tentu akurat. Data cleaning juga perlu dilakukan secara manual untuk beberapa kasus seperti penghapusan link.</t>
+  </si>
+  <si>
+    <t>Untuk pembuatan aplikasi, perlu dibuat secara modular sehingga untuk perubahan ataupun penambahan data pada triplestore tidak akan merubah aplikasi secara keseluruhan. Tahap berikutnya adalah menyempurnakan aplikasi lebih lanjut (meski tetap mungkin terdapat kekurangan) agar dapat digunakan oleh user. Penilaian user lebih berfokus pada aspek kualitas aplikasi dalam mengeksplor data sejarah meskipun validitas data yang digunakan tidak sepenuhnya dapat dipercaya.</t>
+  </si>
+  <si>
+    <t>TODO:
+- Melanjutkan pembuatan aplikasi, khususnya pada frontend agar dapat digunakan oleh user.
+- Melanjutkan pembuatan triple untuk infobox lain untuk data orde baru serta template yang dapat digunakan pada OpenRefine.</t>
+  </si>
+  <si>
+    <t>Alokasi waktu: 16 jam 
+Link Commit: https://github.com/rcsenlia/Ontologi-Sejarah-Indonesia/commit/d8aa2484ad18510cb5c1efa50e9e5920d00133cd
+Uraian:
+- Mengeksplorasi dan mengunduh GraphDB untuk digunakan sebagai triplestore dalam membangun aplikasi
+- Membuat repository backend (https://github.com/ariiesaka/ontologi-sejarah-indonesia-backend) serta mengimplementasikan API untuk mengambil data lokasi dari triplestore dan mengubahnya menjadi data yang dibutuhkan oleh frontend.
+- Meng-clone repository frontend untuk mengintegrasi fitur map dan melakukan pemanggilan terhadap API yang telah dibuat pada backend untuk menampilkan lokasi peristiwa pada peta.
+- Membangun model ontologi dengan memanfaatkan SEM, time, dan GeoSPARQL berdasarkan data yang diperoleh (https://docs.google.com/document/d/1JYA-m2Pb6AzoBysklPjG7AnTKla-Ha_N-EgcU4SmtSk/edit?usp=sharing)
+- Membangun data triple untuk data military conflict pada masa orde baru serta template untuk digunakan pada OpenRefine.
+- Mengeksplorasi library geopy untuk mendapatkan lokasi latitude dan langitude peristiwa berdasarkan lokasi string yang ada pada data.</t>
   </si>
 </sst>
 </file>
@@ -1526,10 +1548,10 @@
   <dimension ref="A1:AE1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="8" topLeftCell="G13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="8" topLeftCell="I13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="K14" sqref="K14"/>
+      <selection pane="bottomRight" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1539,8 +1561,8 @@
     <col min="3" max="3" width="7.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="11" width="40.7109375" customWidth="1"/>
-    <col min="12" max="20" width="17.85546875" customWidth="1"/>
+    <col min="6" max="12" width="40.7109375" customWidth="1"/>
+    <col min="13" max="20" width="17.85546875" customWidth="1"/>
     <col min="21" max="21" width="19.28515625" customWidth="1"/>
     <col min="22" max="23" width="16.5703125" customWidth="1"/>
   </cols>
@@ -2076,7 +2098,9 @@
       <c r="K12" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="L12" s="24"/>
+      <c r="L12" s="24" t="s">
+        <v>141</v>
+      </c>
       <c r="M12" s="24"/>
       <c r="N12" s="24"/>
       <c r="O12" s="24"/>
@@ -2123,7 +2147,9 @@
       <c r="K13" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="L13" s="24"/>
+      <c r="L13" s="24" t="s">
+        <v>142</v>
+      </c>
       <c r="M13" s="24"/>
       <c r="N13" s="24"/>
       <c r="O13" s="24"/>
@@ -2173,7 +2199,7 @@
         <v>139</v>
       </c>
       <c r="L14" s="23" t="s">
-        <v>32</v>
+        <v>144</v>
       </c>
       <c r="M14" s="23" t="s">
         <v>32</v>
@@ -2233,7 +2259,9 @@
         <v>136</v>
       </c>
       <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
+      <c r="L15" s="24" t="s">
+        <v>143</v>
+      </c>
       <c r="M15" s="24"/>
       <c r="N15" s="24"/>
       <c r="O15" s="24"/>

</xml_diff>

<commit_message>
Update the monitoring form for the eight week dated 20/03/2024
</commit_message>
<xml_diff>
--- a/JudahAriesakaMagaini/Judah.xlsx
+++ b/JudahAriesakaMagaini/Judah.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kuliah\semester 8\ta\Ontologi-Sejarah-Indonesia\JudahAriesakaMagaini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA3352D-0A75-4EE8-821E-4739BF4083C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694DD643-266F-4FE9-B07B-5EC42DDFDA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="149">
   <si>
     <t>Monitoring Skripsi dari:</t>
   </si>
@@ -639,6 +639,27 @@
 - Membangun model ontologi dengan memanfaatkan SEM, time, dan GeoSPARQL berdasarkan data yang diperoleh (https://docs.google.com/document/d/1JYA-m2Pb6AzoBysklPjG7AnTKla-Ha_N-EgcU4SmtSk/edit?usp=sharing)
 - Membangun data triple untuk data military conflict pada masa orde baru serta template untuk digunakan pada OpenRefine.
 - Mengeksplorasi library geopy untuk mendapatkan lokasi latitude dan langitude peristiwa berdasarkan lokasi string yang ada pada data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alokasi waktu: 18 jam 
+Link Commit:
+ https://github.com/rcsenlia/fe-ontologi-sejarah-indonesia/commit/dc6563392e3cb065a050dab54c7368e4d83614a5
+https://github.com/ariiesaka/ontologi-sejarah-indonesia-backend/commit/bb6283881cf1813fccad54a54f7b9be9f40da529
+Uraian:
+- Mengimplementasikan halaman detail (frontend) sementara untuk Event
+- Mengimplementasikan API (backend) untuk mengambil data detail Event dari triplestore
+</t>
+  </si>
+  <si>
+    <t>TODO:
+- Melanjutkan pembuatan aplikasi dari sisi frontend
+- Mengintegrasikan data satu sama lain agar aplikasi dapat digunakan</t>
+  </si>
+  <si>
+    <t>Pembuatan aplikasi harus segera diselesaikan agar dapat lanjut ke tahap UAT. Untuk data juga harus segera diintegrasikan satu sama lain.</t>
+  </si>
+  <si>
+    <t>Implementasi frontend cukup kesulitan karena belum terbiasa sehingga memerlukan waktu lebih untuk eksplorasi dan implementasi.</t>
   </si>
 </sst>
 </file>
@@ -1548,10 +1569,10 @@
   <dimension ref="A1:AE1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="8" topLeftCell="I13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="8" topLeftCell="J9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomRight" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1561,8 +1582,8 @@
     <col min="3" max="3" width="7.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="12" width="40.7109375" customWidth="1"/>
-    <col min="13" max="20" width="17.85546875" customWidth="1"/>
+    <col min="6" max="13" width="40.7109375" customWidth="1"/>
+    <col min="14" max="20" width="17.85546875" customWidth="1"/>
     <col min="21" max="21" width="19.28515625" customWidth="1"/>
     <col min="22" max="23" width="16.5703125" customWidth="1"/>
   </cols>
@@ -2101,7 +2122,9 @@
       <c r="L12" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="M12" s="24"/>
+      <c r="M12" s="24" t="s">
+        <v>148</v>
+      </c>
       <c r="N12" s="24"/>
       <c r="O12" s="24"/>
       <c r="P12" s="24"/>
@@ -2150,7 +2173,9 @@
       <c r="L13" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="M13" s="24"/>
+      <c r="M13" s="24" t="s">
+        <v>147</v>
+      </c>
       <c r="N13" s="24"/>
       <c r="O13" s="24"/>
       <c r="P13" s="24"/>
@@ -2202,7 +2227,7 @@
         <v>144</v>
       </c>
       <c r="M14" s="23" t="s">
-        <v>32</v>
+        <v>145</v>
       </c>
       <c r="N14" s="23" t="s">
         <v>32</v>
@@ -2262,7 +2287,9 @@
       <c r="L15" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="M15" s="24"/>
+      <c r="M15" s="24" t="s">
+        <v>146</v>
+      </c>
       <c r="N15" s="24"/>
       <c r="O15" s="24"/>
       <c r="P15" s="24"/>

</xml_diff>

<commit_message>
Update the monitoring form for the ninth week dated 27/03/2024
</commit_message>
<xml_diff>
--- a/JudahAriesakaMagaini/Judah.xlsx
+++ b/JudahAriesakaMagaini/Judah.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kuliah\semester 8\ta\Ontologi-Sejarah-Indonesia\JudahAriesakaMagaini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694DD643-266F-4FE9-B07B-5EC42DDFDA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A6CCE0-F6EA-4612-A84D-584F3903C8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="152">
   <si>
     <t>Monitoring Skripsi dari:</t>
   </si>
@@ -660,6 +660,26 @@
   </si>
   <si>
     <t>Implementasi frontend cukup kesulitan karena belum terbiasa sehingga memerlukan waktu lebih untuk eksplorasi dan implementasi.</t>
+  </si>
+  <si>
+    <t>Alokasi waktu: 18 jam
+Link Commit:
+https://github.com/rcsenlia/Ontologi-Sejarah-Indonesia/commit/a34b627a6579e781d2f8ad00f1c4973d2b09468f
+https://github.com/rcsenlia/Ontologi-Sejarah-Indonesia/commit/69f2cbc0b05bcf3be82d863fa51db9bc1849c5d3
+https://github.com/rcsenlia/fe-ontologi-sejarah-indonesia/commit/ae1d3d9d01b582ff4cc4a1a04ad09a91cf9e107f
+https://github.com/ariiesaka/ontologi-sejarah-indonesia-backend/commit/9b6e8e30593306fbbe24923df6e9b8a3c299e913
+Uraian:
+- Melakukan perbaikan pada data agar dapat diintegrasikan pada aplikasi untuk seluruh fitur timeline, map, dan graph
+- Memperbaiki dan melengkapi implementasi kode backend untuk detail agar lebih modular terhadap perubahan data
+- Memperbaiki dan melengkapi implementasi kode frontend untuk tampilan map dan detail</t>
+  </si>
+  <si>
+    <t>TODO:
+- Melakukan perbaikan pada tampilan frontend map dan detail
+- Menambah serta mengintegrasikan data satu sama lain untuk meningkatkan usability aplikasi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Untuk tampilan frontend perlu diperbaiki agar lebih intuitif bagi pengguna seperti penambahan fitur search dan filter berdasarkan waktu, font yang lebih besar, layout detail yang lebih baik dan sebagainya. Agar ontologi lebih kaya, dapat menggunakan ontologi dari dublincore dcterms. Selanjutnya, perlu didiskusikan dengan pihak sejarah mengenai rancangan ontologi yang telah dibuat. </t>
   </si>
 </sst>
 </file>
@@ -1569,10 +1589,10 @@
   <dimension ref="A1:AE1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="8" topLeftCell="J9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="8" topLeftCell="K9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="M13" sqref="M13"/>
+      <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1582,8 +1602,8 @@
     <col min="3" max="3" width="7.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="13" width="40.7109375" customWidth="1"/>
-    <col min="14" max="20" width="17.85546875" customWidth="1"/>
+    <col min="6" max="14" width="40.7109375" customWidth="1"/>
+    <col min="15" max="20" width="17.85546875" customWidth="1"/>
     <col min="21" max="21" width="19.28515625" customWidth="1"/>
     <col min="22" max="23" width="16.5703125" customWidth="1"/>
   </cols>
@@ -2125,7 +2145,9 @@
       <c r="M12" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="N12" s="24"/>
+      <c r="N12" s="24" t="s">
+        <v>123</v>
+      </c>
       <c r="O12" s="24"/>
       <c r="P12" s="24"/>
       <c r="Q12" s="24"/>
@@ -2176,7 +2198,9 @@
       <c r="M13" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="N13" s="24"/>
+      <c r="N13" s="24" t="s">
+        <v>151</v>
+      </c>
       <c r="O13" s="24"/>
       <c r="P13" s="24"/>
       <c r="Q13" s="24"/>
@@ -2230,7 +2254,7 @@
         <v>145</v>
       </c>
       <c r="N14" s="23" t="s">
-        <v>32</v>
+        <v>149</v>
       </c>
       <c r="O14" s="23" t="s">
         <v>32</v>
@@ -2290,7 +2314,9 @@
       <c r="M15" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="N15" s="24"/>
+      <c r="N15" s="24" t="s">
+        <v>150</v>
+      </c>
       <c r="O15" s="24"/>
       <c r="P15" s="24"/>
       <c r="Q15" s="24"/>

</xml_diff>

<commit_message>
Update the monitoring form for the tenth week dated 03/04/2024
</commit_message>
<xml_diff>
--- a/JudahAriesakaMagaini/Judah.xlsx
+++ b/JudahAriesakaMagaini/Judah.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kuliah\semester 8\ta\Ontologi-Sejarah-Indonesia\JudahAriesakaMagaini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A6CCE0-F6EA-4612-A84D-584F3903C8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371617EB-CDCC-453D-98F6-05B832F555FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="155">
   <si>
     <t>Monitoring Skripsi dari:</t>
   </si>
@@ -680,6 +680,28 @@
   </si>
   <si>
     <t xml:space="preserve">Untuk tampilan frontend perlu diperbaiki agar lebih intuitif bagi pengguna seperti penambahan fitur search dan filter berdasarkan waktu, font yang lebih besar, layout detail yang lebih baik dan sebagainya. Agar ontologi lebih kaya, dapat menggunakan ontologi dari dublincore dcterms. Selanjutnya, perlu didiskusikan dengan pihak sejarah mengenai rancangan ontologi yang telah dibuat. </t>
+  </si>
+  <si>
+    <t>TODO:
+- Membuat skenario tes UT dan UAT
+- Melengkapi keseluruhan data dan mengintegrasikan data untuk meningkatkan usability aplikasi
+- Memperbaiki aplikasi sesuai input Bu Isye (menghapus search bar dari navbar serta memperbaiki tampilan dan fungsionalitas search bar)</t>
+  </si>
+  <si>
+    <t>Alokasi waktu: 18 jam
+Link Commit:
+https://github.com/rcsenlia/fe-ontologi-sejarah-indonesia/commit/3a1a93973f8536067409d6ae4289ecc32e47f5f1
+https://github.com/rcsenlia/fe-ontologi-sejarah-indonesia/commit/cd70a84d8768c667702e896f29199e006a611f52
+https://github.com/ariiesaka/ontologi-sejarah-indonesia-backend/commit/5d622d704af30adbc7e1969dea77e695b6a05de6
+Uraian:
+- Menambahkan fitur search untuk melakukan pencarian detail pada actor, event, dan place pada navbar
+- Menambahkan fitur filter event pada peta berdasarkan input yang diketikkan user
+- Memperbaiki tampilan frontend, khususnya search bar dan suggestions
+- Mengimplementasikan API untuk mengembalikan hasil search dan memperbaiki API untuk mengembalikan hasil detail
+- Menunjukkan prototype aplikasi dan menerima masukan untuk diperbaiki untuk pekan yang akan datang</t>
+  </si>
+  <si>
+    <t>Terdapat 2 search bar yang membuat aplikasi kurang intuitif sehingga akan dihapus salah satu. Aplikasi akan dikembangkan sesuai dengan arahan dan masukan Bu Isye untuk kemudian akan dilakukan UT dan UAT ketika telah selesai. Aplikasi dan data harus sudah selesai setelah libur lebaran.</t>
   </si>
 </sst>
 </file>
@@ -1589,10 +1611,10 @@
   <dimension ref="A1:AE1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="8" topLeftCell="K9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="8" topLeftCell="M9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
+      <selection pane="bottomRight" activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1602,8 +1624,8 @@
     <col min="3" max="3" width="7.42578125" customWidth="1"/>
     <col min="4" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="14" width="40.7109375" customWidth="1"/>
-    <col min="15" max="20" width="17.85546875" customWidth="1"/>
+    <col min="6" max="15" width="40.7109375" customWidth="1"/>
+    <col min="16" max="20" width="17.85546875" customWidth="1"/>
     <col min="21" max="21" width="19.28515625" customWidth="1"/>
     <col min="22" max="23" width="16.5703125" customWidth="1"/>
   </cols>
@@ -2148,7 +2170,9 @@
       <c r="N12" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="O12" s="24"/>
+      <c r="O12" s="24" t="s">
+        <v>123</v>
+      </c>
       <c r="P12" s="24"/>
       <c r="Q12" s="24"/>
       <c r="R12" s="25"/>
@@ -2201,7 +2225,9 @@
       <c r="N13" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="O13" s="24"/>
+      <c r="O13" s="24" t="s">
+        <v>154</v>
+      </c>
       <c r="P13" s="24"/>
       <c r="Q13" s="24"/>
       <c r="R13" s="25"/>
@@ -2257,7 +2283,7 @@
         <v>149</v>
       </c>
       <c r="O14" s="23" t="s">
-        <v>32</v>
+        <v>153</v>
       </c>
       <c r="P14" s="23" t="s">
         <v>32</v>
@@ -2317,7 +2343,9 @@
       <c r="N15" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="O15" s="24"/>
+      <c r="O15" s="24" t="s">
+        <v>152</v>
+      </c>
       <c r="P15" s="24"/>
       <c r="Q15" s="24"/>
       <c r="R15" s="25"/>

</xml_diff>

<commit_message>
Update the monitoring form for the eleventh week dated 17/04/2024
</commit_message>
<xml_diff>
--- a/JudahAriesakaMagaini/Judah.xlsx
+++ b/JudahAriesakaMagaini/Judah.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kuliah\semester 8\ta\Ontologi-Sejarah-Indonesia\JudahAriesakaMagaini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371617EB-CDCC-453D-98F6-05B832F555FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4735DAAF-C9A0-4B46-B69C-4BB52D74D284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="158">
   <si>
     <t>Monitoring Skripsi dari:</t>
   </si>
@@ -702,6 +702,25 @@
   </si>
   <si>
     <t>Terdapat 2 search bar yang membuat aplikasi kurang intuitif sehingga akan dihapus salah satu. Aplikasi akan dikembangkan sesuai dengan arahan dan masukan Bu Isye untuk kemudian akan dilakukan UT dan UAT ketika telah selesai. Aplikasi dan data harus sudah selesai setelah libur lebaran.</t>
+  </si>
+  <si>
+    <t>Alokasi waktu: 18 jam
+Link Commit: ....
+https://github.com/rcsenlia/fe-ontologi-sejarah-indonesia/commit/06b91e098f3ba33b746e5c1723c13ff2e5aa2321
+https://github.com/ariiesaka/ontologi-sejarah-indonesia-backend/commit/a95e5c296e75bf0d4e168804632c85144dc9b534
+Uraian:
+- Memperbaiki halaman visualisasi peta dimana suatu lokasi (latitude dan longitude) bisa saja memiliki lebih dari satu peristiwa
+- Memperbaiki API yang mengembalikan data peristiwa untuk ditampilkan pada peta
+- Mengumpulkan dan membersihkan data untuk office holder</t>
+  </si>
+  <si>
+    <t>TODO:
+- Membuat skenario tes UT
+- Melengkapi keseluruhan data dan mengintegrasikan data untuk meningkatkan usability aplikasi
+- Mengimplementasi halaman pencarian lebih lanjut</t>
+  </si>
+  <si>
+    <t>Tulisan pada aplikasi perlu dibuat lebih besar untuk memudahkan user. Selain itu, perlu diimplementasikan fitur pencarian lebih lanjut agar user tidak melakukan scrolling pada search bar. Mulai mengerjakan Bab 1 untuk menentukan tes yang akan digunakan untuk menilai aplikasi.</t>
   </si>
 </sst>
 </file>
@@ -1614,7 +1633,7 @@
       <pane xSplit="4" ySplit="8" topLeftCell="M9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="P13" sqref="P13"/>
+      <selection pane="bottomRight" activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1625,7 +1644,9 @@
     <col min="4" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
     <col min="6" max="15" width="40.7109375" customWidth="1"/>
-    <col min="16" max="20" width="17.85546875" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" customWidth="1"/>
+    <col min="17" max="17" width="40.7109375" customWidth="1"/>
+    <col min="18" max="20" width="17.85546875" customWidth="1"/>
     <col min="21" max="21" width="19.28515625" customWidth="1"/>
     <col min="22" max="23" width="16.5703125" customWidth="1"/>
   </cols>
@@ -2174,7 +2195,9 @@
         <v>123</v>
       </c>
       <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
+      <c r="Q12" s="24" t="s">
+        <v>123</v>
+      </c>
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
       <c r="T12" s="25"/>
@@ -2229,7 +2252,9 @@
         <v>154</v>
       </c>
       <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
+      <c r="Q13" s="24" t="s">
+        <v>157</v>
+      </c>
       <c r="R13" s="25"/>
       <c r="S13" s="25"/>
       <c r="T13" s="25"/>
@@ -2289,7 +2314,7 @@
         <v>32</v>
       </c>
       <c r="Q14" s="23" t="s">
-        <v>32</v>
+        <v>155</v>
       </c>
       <c r="R14" s="23" t="s">
         <v>32</v>
@@ -2347,7 +2372,9 @@
         <v>152</v>
       </c>
       <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
+      <c r="Q15" s="24" t="s">
+        <v>156</v>
+      </c>
       <c r="R15" s="25"/>
       <c r="S15" s="25"/>
       <c r="T15" s="25"/>

</xml_diff>

<commit_message>
Update the monitoring form for the twelfth week dated 24/04/2024
</commit_message>
<xml_diff>
--- a/JudahAriesakaMagaini/Judah.xlsx
+++ b/JudahAriesakaMagaini/Judah.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kuliah\semester 8\ta\Ontologi-Sejarah-Indonesia\JudahAriesakaMagaini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4735DAAF-C9A0-4B46-B69C-4BB52D74D284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC7F2FE5-C33E-439D-AA20-16C1A0C34374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="161">
   <si>
     <t>Monitoring Skripsi dari:</t>
   </si>
@@ -721,6 +721,26 @@
   </si>
   <si>
     <t>Tulisan pada aplikasi perlu dibuat lebih besar untuk memudahkan user. Selain itu, perlu diimplementasikan fitur pencarian lebih lanjut agar user tidak melakukan scrolling pada search bar. Mulai mengerjakan Bab 1 untuk menentukan tes yang akan digunakan untuk menilai aplikasi.</t>
+  </si>
+  <si>
+    <t>Alokasi waktu: 18 jam
+Link Commit:
+https://github.com/rcsenlia/fe-ontologi-sejarah-indonesia/commit/89b341f1d72f5b93a26904873dfbe053d5bc497a
+https://docs.google.com/document/d/1d2mRMccbpBjg6NLmSGD0AVug6UralHHyPygsQs5fYvk/edit?usp=sharing
+https://docs.google.com/document/d/1hkAfbXqfVFserj2wXsMK94FCP9jldHQ-/edit?usp=sharing&amp;ouid=101855055134988115118&amp;rtpof=true&amp;sd=true
+Uraian:
+- Memperbesar ukuran font dan popup pada halaman Peta
+- Mulai menulis Bab 1 yang meliputi latar belakang, rumusan masalah, tujuan penelitian, manfaat penelitian, ruang lingkup penelitian, dan sistematika penulisan.
+- Mulai menulis Bab 4 yang berisi metodologi pembuatan visualisasi peta
+- Membuat skenario tes UT untuk halaman visualisasi Peta dan detail</t>
+  </si>
+  <si>
+    <t>TODO:
+- Melanjutkan penulisan laporan
+- Melengkapi keseluruhan data</t>
+  </si>
+  <si>
+    <t>Dosen pembimbing memberi banyak masukan pada tulisan Bab 1 yang telah dibuat, terutama pada latar belakang, rumusan penelitian, ruang lingkup penelitian, dan sistematika penulisan. Langkah selanjutnya adalah mendeploy aplikasi untuk dilakukan UAT. Perlu dibuat rencana lain agar UAT dapat dijalankan lebih cepat.</t>
   </si>
 </sst>
 </file>
@@ -1630,10 +1650,10 @@
   <dimension ref="A1:AE1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="8" topLeftCell="M9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="8" topLeftCell="N9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="O13" sqref="O13"/>
+      <selection pane="bottomRight" activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1645,8 +1665,8 @@
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
     <col min="6" max="15" width="40.7109375" customWidth="1"/>
     <col min="16" max="16" width="17.85546875" customWidth="1"/>
-    <col min="17" max="17" width="40.7109375" customWidth="1"/>
-    <col min="18" max="20" width="17.85546875" customWidth="1"/>
+    <col min="17" max="18" width="40.7109375" customWidth="1"/>
+    <col min="19" max="20" width="17.85546875" customWidth="1"/>
     <col min="21" max="21" width="19.28515625" customWidth="1"/>
     <col min="22" max="23" width="16.5703125" customWidth="1"/>
   </cols>
@@ -2198,7 +2218,9 @@
       <c r="Q12" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="R12" s="25"/>
+      <c r="R12" s="25" t="s">
+        <v>123</v>
+      </c>
       <c r="S12" s="25"/>
       <c r="T12" s="25"/>
       <c r="U12" s="25"/>
@@ -2255,7 +2277,9 @@
       <c r="Q13" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="R13" s="25"/>
+      <c r="R13" s="24" t="s">
+        <v>160</v>
+      </c>
       <c r="S13" s="25"/>
       <c r="T13" s="25"/>
       <c r="U13" s="25"/>
@@ -2317,7 +2341,7 @@
         <v>155</v>
       </c>
       <c r="R14" s="23" t="s">
-        <v>32</v>
+        <v>158</v>
       </c>
       <c r="S14" s="23" t="s">
         <v>32</v>
@@ -2375,7 +2399,9 @@
       <c r="Q15" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="R15" s="25"/>
+      <c r="R15" s="24" t="s">
+        <v>159</v>
+      </c>
       <c r="S15" s="25"/>
       <c r="T15" s="25"/>
       <c r="U15" s="25"/>

</xml_diff>